<commit_message>
REST with Jersey, Maven, Groovy
REST with Jersey, Maven, Groovy
</commit_message>
<xml_diff>
--- a/Definitions/9_Definitions_Web_Services.xlsx
+++ b/Definitions/9_Definitions_Web_Services.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="278">
   <si>
     <t>Topic</t>
   </si>
@@ -1370,6 +1370,18 @@
       </rPr>
       <t xml:space="preserve"> annotation to pojo at class level</t>
     </r>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Bad Request (Missing Information</t>
+  </si>
+  <si>
+    <t>400 response code</t>
+  </si>
+  <si>
+    <t>200  response code</t>
   </si>
 </sst>
 </file>
@@ -3261,11 +3273,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3364,6 +3376,22 @@
       </c>
       <c r="B14" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B16" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>